<commit_message>
Har sammanfattat vad jag gjort för att skicka till NH.
</commit_message>
<xml_diff>
--- a/reports/table1.xlsx
+++ b/reports/table1.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C95"/>
+  <dimension ref="A1:C96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -389,41 +389,41 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>P_Age (mean (sd))</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>68.79 (9.93)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>P_Gender (%)</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Man</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">30522 (44.3) </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
         <is>
           <t>Kvinna</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t xml:space="preserve">38337 (55.7) </t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Man</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">30522 (44.3) </t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>P_Age (mean (sd))</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>68.79 (9.93)</t>
         </is>
       </c>
     </row>
@@ -442,1108 +442,1120 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>education (%)</t>
+          <t>P_ASA (%)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>high</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">17671 (25.7) </t>
+          <t xml:space="preserve">16784 (24.4) </t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="inlineStr">
         <is>
-          <t>low</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">22815 (33.1) </t>
+          <t xml:space="preserve">41294 (60.0) </t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="inlineStr">
         <is>
-          <t>middle</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">28373 (41.2) </t>
+          <t xml:space="preserve">10781 (15.7) </t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>civil_status (%)</t>
+          <t>P_TypeOfHospital (%)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>married</t>
+          <t>Universitets- eller regionssjukhus</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">38972 (56.6) </t>
+          <t xml:space="preserve"> 4750 ( 6.9) </t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="inlineStr">
         <is>
-          <t>single</t>
+          <t>Länsdelsjukhus</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">19326 (28.1) </t>
+          <t xml:space="preserve">27698 (40.2) </t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="inlineStr">
         <is>
-          <t>widow/widower</t>
+          <t>Länssjukhus</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">10561 (15.3) </t>
+          <t xml:space="preserve">21732 (31.6) </t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>P_ASA (%)</t>
-        </is>
-      </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Privatsjukhus</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">16784 (24.4) </t>
+          <t xml:space="preserve">14679 (21.3) </t>
         </is>
       </c>
     </row>
     <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>P_ProtGrp (%)</t>
+        </is>
+      </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>Cemented</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve">41294 (60.0) </t>
+          <t xml:space="preserve">46115 (67.0) </t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>Cementless</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">10781 (15.7) </t>
+          <t xml:space="preserve">11731 (17.0) </t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>elix_icd10_index_walraven (%)</t>
-        </is>
-      </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>-14</t>
+          <t>Hybrid</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1 ( 0.0) </t>
+          <t xml:space="preserve"> 1929 ( 2.8) </t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="inlineStr">
         <is>
-          <t>-11</t>
+          <t>Reversed hybrid</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1 ( 0.0) </t>
+          <t xml:space="preserve"> 9084 (13.2) </t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>-10</t>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>P_SurgYear (mean (sd))</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">   10 ( 0.0) </t>
+          <t xml:space="preserve"> 3.74 (2.26)</t>
         </is>
       </c>
     </row>
     <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>education (%)</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>-7</t>
+          <t>low</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">   38 ( 0.1) </t>
+          <t xml:space="preserve">22815 (33.1) </t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="inlineStr">
         <is>
-          <t>-6</t>
+          <t>high</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve">    5 ( 0.0) </t>
+          <t xml:space="preserve">17671 (25.7) </t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="inlineStr">
         <is>
-          <t>-5</t>
+          <t>middle</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">   15 ( 0.0) </t>
+          <t xml:space="preserve">28373 (41.2) </t>
         </is>
       </c>
     </row>
     <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>civil_status (%)</t>
+        </is>
+      </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>-4</t>
+          <t>married</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve">  416 ( 0.6) </t>
+          <t xml:space="preserve">38972 (56.6) </t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="inlineStr">
         <is>
-          <t>-3</t>
+          <t>single</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">  342 ( 0.5) </t>
+          <t xml:space="preserve">19326 (28.1) </t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="inlineStr">
         <is>
-          <t>-2</t>
+          <t>widow/widower</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve">  123 ( 0.2) </t>
+          <t xml:space="preserve">10561 (15.3) </t>
         </is>
       </c>
     </row>
     <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>ECI_index_walraven (%)</t>
+        </is>
+      </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>-1</t>
+          <t>-14</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve">  406 ( 0.6) </t>
+          <t xml:space="preserve">    1 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-11</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve">61121 (88.8) </t>
+          <t xml:space="preserve">    1 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>-10</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve">  107 ( 0.2) </t>
+          <t xml:space="preserve">   10 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>-7</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve">  230 ( 0.3) </t>
+          <t xml:space="preserve">   38 ( 0.1) </t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>-6</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1148 ( 1.7) </t>
+          <t xml:space="preserve">    5 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>-5</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1126 ( 1.6) </t>
+          <t xml:space="preserve">   15 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>-4</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1769 ( 2.6) </t>
+          <t xml:space="preserve">  416 ( 0.6) </t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>-3</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t xml:space="preserve">  339 ( 0.5) </t>
+          <t xml:space="preserve">  342 ( 0.5) </t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>-2</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve">  370 ( 0.5) </t>
+          <t xml:space="preserve">  123 ( 0.2) </t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t xml:space="preserve">  161 ( 0.2) </t>
+          <t xml:space="preserve">  406 ( 0.6) </t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve">  239 ( 0.3) </t>
+          <t xml:space="preserve">61121 (88.8) </t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t xml:space="preserve">  112 ( 0.2) </t>
+          <t xml:space="preserve">  107 ( 0.2) </t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t xml:space="preserve">  164 ( 0.2) </t>
+          <t xml:space="preserve">  230 ( 0.3) </t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t xml:space="preserve">  285 ( 0.4) </t>
+          <t xml:space="preserve"> 1148 ( 1.7) </t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t xml:space="preserve">   30 ( 0.0) </t>
+          <t xml:space="preserve"> 1126 ( 1.6) </t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t xml:space="preserve">   49 ( 0.1) </t>
+          <t xml:space="preserve"> 1769 ( 2.6) </t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t xml:space="preserve">   46 ( 0.1) </t>
+          <t xml:space="preserve">  339 ( 0.5) </t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>7</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t xml:space="preserve">   93 ( 0.1) </t>
+          <t xml:space="preserve">  370 ( 0.5) </t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>8</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t xml:space="preserve">   41 ( 0.1) </t>
+          <t xml:space="preserve">  161 ( 0.2) </t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>9</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t xml:space="preserve">   13 ( 0.0) </t>
+          <t xml:space="preserve">  239 ( 0.3) </t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t xml:space="preserve">   15 ( 0.0) </t>
+          <t xml:space="preserve">  112 ( 0.2) </t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t xml:space="preserve">   12 ( 0.0) </t>
+          <t xml:space="preserve">  164 ( 0.2) </t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t xml:space="preserve">   16 ( 0.0) </t>
+          <t xml:space="preserve">  285 ( 0.4) </t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>13</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t xml:space="preserve">    4 ( 0.0) </t>
+          <t xml:space="preserve">   30 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>14</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t xml:space="preserve">    2 ( 0.0) </t>
+          <t xml:space="preserve">   49 ( 0.1) </t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>15</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t xml:space="preserve">    3 ( 0.0) </t>
+          <t xml:space="preserve">   46 ( 0.1) </t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>16</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1 ( 0.0) </t>
+          <t xml:space="preserve">   93 ( 0.1) </t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>17</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1 ( 0.0) </t>
+          <t xml:space="preserve">   41 ( 0.1) </t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>18</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t xml:space="preserve">    2 ( 0.0) </t>
+          <t xml:space="preserve">   13 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1 ( 0.0) </t>
+          <t xml:space="preserve">   15 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>20</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1 ( 0.0) </t>
+          <t xml:space="preserve">   12 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>21</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1 ( 0.0) </t>
+          <t xml:space="preserve">   16 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>charlson_icd10_index_quan_original (%)</t>
-        </is>
-      </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>22</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t xml:space="preserve">60970 (88.5) </t>
+          <t xml:space="preserve">    4 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>23</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 4691 ( 6.8) </t>
+          <t xml:space="preserve">    2 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2161 ( 3.1) </t>
+          <t xml:space="preserve">    3 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t xml:space="preserve">  609 ( 0.9) </t>
+          <t xml:space="preserve">    1 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>26</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t xml:space="preserve">  195 ( 0.3) </t>
+          <t xml:space="preserve">    1 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>27</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t xml:space="preserve">   88 ( 0.1) </t>
+          <t xml:space="preserve">    2 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>28</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t xml:space="preserve">   40 ( 0.1) </t>
+          <t xml:space="preserve">    1 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>32</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t xml:space="preserve">   14 ( 0.0) </t>
+          <t xml:space="preserve">    1 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>33</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t xml:space="preserve">   60 ( 0.1) </t>
+          <t xml:space="preserve">    1 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>CCI_index_quan_original (%)</t>
+        </is>
+      </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t xml:space="preserve">   23 ( 0.0) </t>
+          <t xml:space="preserve">60970 (88.5) </t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t xml:space="preserve">    2 ( 0.0) </t>
+          <t xml:space="preserve"> 4691 ( 6.8) </t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t xml:space="preserve">    4 ( 0.0) </t>
+          <t xml:space="preserve"> 2161 ( 3.1) </t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t xml:space="preserve">    2 ( 0.0) </t>
+          <t xml:space="preserve">  609 ( 0.9) </t>
         </is>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>rxriskv_modified_atc_index_index (%)</t>
-        </is>
-      </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t xml:space="preserve">35849 (52.1) </t>
+          <t xml:space="preserve">  195 ( 0.3) </t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 4979 ( 7.2) </t>
+          <t xml:space="preserve">   88 ( 0.1) </t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 5437 ( 7.9) </t>
+          <t xml:space="preserve">   40 ( 0.1) </t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 5121 ( 7.4) </t>
+          <t xml:space="preserve">   14 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="B74" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 4718 ( 6.9) </t>
+          <t xml:space="preserve">   60 ( 0.1) </t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="B75" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>9</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 4170 ( 6.1) </t>
+          <t xml:space="preserve">   23 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="B76" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 3297 ( 4.8) </t>
+          <t xml:space="preserve">    2 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="B77" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2326 ( 3.4) </t>
+          <t xml:space="preserve">    4 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="B78" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1422 ( 2.1) </t>
+          <t xml:space="preserve">    2 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Rx_index_index (%)</t>
+        </is>
+      </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t xml:space="preserve">  772 ( 1.1) </t>
+          <t xml:space="preserve">35849 (52.1) </t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="B80" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t xml:space="preserve">  420 ( 0.6) </t>
+          <t xml:space="preserve"> 4979 ( 7.2) </t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="B81" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t xml:space="preserve">  202 ( 0.3) </t>
+          <t xml:space="preserve"> 5437 ( 7.9) </t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="B82" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t xml:space="preserve">   85 ( 0.1) </t>
+          <t xml:space="preserve"> 5121 ( 7.4) </t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="B83" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t xml:space="preserve">   31 ( 0.0) </t>
+          <t xml:space="preserve"> 4718 ( 6.9) </t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="B84" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t xml:space="preserve">   21 ( 0.0) </t>
+          <t xml:space="preserve"> 4170 ( 6.1) </t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="B85" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t xml:space="preserve">    6 ( 0.0) </t>
+          <t xml:space="preserve"> 3297 ( 4.8) </t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="B86" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>7</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t xml:space="preserve">    2 ( 0.0) </t>
+          <t xml:space="preserve"> 2326 ( 3.4) </t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="B87" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>8</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1 ( 0.0) </t>
+          <t xml:space="preserve"> 1422 ( 2.1) </t>
         </is>
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>P_TypeOfHospital (%)</t>
-        </is>
-      </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Länsdelsjukhus</t>
+          <t>9</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t xml:space="preserve">27698 (40.2) </t>
+          <t xml:space="preserve">  772 ( 1.1) </t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="B89" t="inlineStr">
         <is>
-          <t>Länssjukhus</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t xml:space="preserve">21732 (31.6) </t>
+          <t xml:space="preserve">  420 ( 0.6) </t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="B90" t="inlineStr">
         <is>
-          <t>Privatsjukhus</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t xml:space="preserve">14679 (21.3) </t>
+          <t xml:space="preserve">  202 ( 0.3) </t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="B91" t="inlineStr">
         <is>
-          <t>Universitets- eller regionssjukhus</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 4750 ( 6.9) </t>
+          <t xml:space="preserve">   85 ( 0.1) </t>
         </is>
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>P_ProtGrp (%)</t>
-        </is>
-      </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Cemented</t>
+          <t>13</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t xml:space="preserve">46115 (67.0) </t>
+          <t xml:space="preserve">   31 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="B93" t="inlineStr">
         <is>
-          <t>Cementless</t>
+          <t>14</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t xml:space="preserve">11731 (17.0) </t>
+          <t xml:space="preserve">   21 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="B94" t="inlineStr">
         <is>
-          <t>Hybrid</t>
+          <t>15</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1929 ( 2.8) </t>
+          <t xml:space="preserve">    6 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="B95" t="inlineStr">
         <is>
-          <t>Reversed hybrid</t>
+          <t>16</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 9084 (13.2) </t>
+          <t xml:space="preserve">    2 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    1 ( 0.0) </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
new version with correct comorbidity data. See (other project but related): https://www.pivotaltracker.com/story/show/164274282
</commit_message>
<xml_diff>
--- a/reports/table1.xlsx
+++ b/reports/table1.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -389,239 +389,1130 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P_Age (mean (sd))</t>
+          <t>P_ASA (%)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>72.50 (7.79)</t>
+          <t xml:space="preserve"> 8429 (18.3) </t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>P_Gender (%)</t>
-        </is>
-      </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Man</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">18103 (39.3) </t>
+          <t xml:space="preserve">29383 (63.7) </t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>Kvinna</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">28012 (60.7) </t>
+          <t xml:space="preserve"> 8303 (18.0) </t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P_BMI (mean (sd))</t>
+          <t>ECI_index_walraven (%)</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>-11</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>27.17 (4.38)</t>
+          <t xml:space="preserve">    1 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>P_ASA (%)</t>
-        </is>
-      </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>-10</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 8429 (18.3) </t>
+          <t xml:space="preserve">    8 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>-7</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">29383 (63.7) </t>
+          <t xml:space="preserve">   31 ( 0.1) </t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>-6</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 8303 (18.0) </t>
+          <t xml:space="preserve">    9 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>P_TypeOfHospital (%)</t>
-        </is>
-      </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Universitets- eller regionssjukhus</t>
+          <t>-5</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1875 ( 4.1) </t>
+          <t xml:space="preserve">   22 ( 0.0) </t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="inlineStr">
         <is>
-          <t>Länsdelsjukhus</t>
+          <t>-4</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">21273 (46.1) </t>
+          <t xml:space="preserve">  495 ( 1.1) </t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="inlineStr">
         <is>
-          <t>Länssjukhus</t>
+          <t>-3</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">14263 (30.9) </t>
+          <t xml:space="preserve">  402 ( 0.9) </t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="inlineStr">
         <is>
-          <t>Privatsjukhus</t>
+          <t>-2</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 8704 (18.9) </t>
+          <t xml:space="preserve">  204 ( 0.4) </t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>P_SurgYear (mean (sd))</t>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>-1</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 4.59 (2.26)</t>
+          <t xml:space="preserve">  596 ( 1.3) </t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>education (%)</t>
-        </is>
-      </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>low</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">17913 (38.8) </t>
+          <t xml:space="preserve">34864 (75.6) </t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="inlineStr">
         <is>
-          <t>high</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">10095 (21.9) </t>
+          <t xml:space="preserve">  137 ( 0.3) </t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="inlineStr">
         <is>
-          <t>middle</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">18107 (39.3) </t>
+          <t xml:space="preserve">  366 ( 0.8) </t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>civil_status (%)</t>
-        </is>
-      </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>married</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">25676 (55.7) </t>
+          <t xml:space="preserve"> 1620 ( 3.5) </t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="inlineStr">
         <is>
-          <t>single</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">11193 (24.3) </t>
+          <t xml:space="preserve"> 1687 ( 3.7) </t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="inlineStr">
         <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2583 ( 5.6) </t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  481 ( 1.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  575 ( 1.2) </t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  274 ( 0.6) </t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  352 ( 0.8) </t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  167 ( 0.4) </t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  238 ( 0.5) </t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  453 ( 1.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   47 ( 0.1) </t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   91 ( 0.2) </t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   85 ( 0.2) </t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  165 ( 0.4) </t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   49 ( 0.1) </t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   17 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   24 ( 0.1) </t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   17 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   28 ( 0.1) </t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    9 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    5 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    3 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    2 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    1 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    2 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    2 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    1 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    1 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    1 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>CCI_index_quan_original (%)</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">34239 (74.2) </t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6952 (15.1) </t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3229 ( 7.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  999 ( 2.2) </t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  330 ( 0.7) </t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  133 ( 0.3) </t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   62 ( 0.1) </t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   16 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  108 ( 0.2) </t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   32 ( 0.1) </t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    5 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    4 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    5 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    1 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Rx_index_index (%)</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2697 ( 5.8) </t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5275 (11.4) </t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6455 (14.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6688 (14.5) </t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6439 (14.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5842 (12.7) </t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4881 (10.6) </t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3368 ( 7.3) </t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2085 ( 4.5) </t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1209 ( 2.6) </t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  648 ( 1.4) </t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  298 ( 0.6) </t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  139 ( 0.3) </t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   54 ( 0.1) </t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   24 ( 0.1) </t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    8 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    3 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    2 ( 0.0) </t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>P_Age (mean (SD))</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>72.50 (7.79)</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>P_Gender (%)</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Man</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">18103 (39.3) </t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Kvinna</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">28012 (60.7) </t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>P_BMI (mean (SD))</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>27.17 (4.38)</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>P_TypeOfHospital (%)</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Universitets- eller regionssjukhus</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1875 ( 4.1) </t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Länsdelsjukhus</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">21273 (46.1) </t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Länssjukhus</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">14263 (30.9) </t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Privatsjukhus</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8704 (18.9) </t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>P_SurgYear (mean (SD))</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4.59 (2.26)</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>education (%)</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">17913 (38.8) </t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10095 (21.9) </t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>middle</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">18107 (39.3) </t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>civil_status (%)</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>married</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">25676 (55.7) </t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">11193 (24.3) </t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93" t="inlineStr">
+        <is>
           <t>widow/widower</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C93" t="inlineStr">
         <is>
           <t xml:space="preserve"> 9246 (20.0) </t>
         </is>

</xml_diff>